<commit_message>
Checkin and Environment stuff
</commit_message>
<xml_diff>
--- a/Project Checkout Sheet.xlsx
+++ b/Project Checkout Sheet.xlsx
@@ -104,7 +104,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[h]&quot;h&quot;"/>
+    <numFmt numFmtId="166" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -407,24 +407,14 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -491,6 +481,17 @@
     </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1822,515 +1823,517 @@
   <dimension ref="A1:IV33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.8984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.59765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" style="32" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="32" customWidth="1"/>
+    <col min="3" max="3" width="17.8984375" style="32" customWidth="1"/>
+    <col min="4" max="4" width="18.59765625" style="32" customWidth="1"/>
     <col min="5" max="256" width="6.59765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="31" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="33"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="27"/>
     </row>
     <row r="2" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="22" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="31">
         <v>0.125</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="31">
         <v>42054.284722222219</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="31">
         <v>42054.395833333336</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="27"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="27"/>
+      <c r="D4" s="31">
+        <v>0.8125</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="27"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="27"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="21"/>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="27"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="21"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="27"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="21"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="27"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="21"/>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="27"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="21"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="27"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="21"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="27"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="21"/>
     </row>
     <row r="13" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="21"/>
     </row>
     <row r="14" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="27"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="21"/>
     </row>
     <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="27"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="21"/>
     </row>
     <row r="16" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="27"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="21"/>
     </row>
     <row r="17" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="27"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="21"/>
     </row>
     <row r="18" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="27"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="21"/>
     </row>
     <row r="19" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="27"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="21"/>
     </row>
     <row r="20" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="21"/>
     </row>
     <row r="21" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="27"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="21"/>
     </row>
     <row r="22" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="30"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="24"/>
     </row>
     <row r="23" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="13" t="s">
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="15"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="9"/>
     </row>
     <row r="26" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="18"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="12"/>
     </row>
     <row r="27" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="18"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="12"/>
     </row>
     <row r="28" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="18"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="12"/>
     </row>
     <row r="29" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="18"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="12"/>
     </row>
     <row r="30" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="18"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="12"/>
     </row>
     <row r="31" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="18"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="12"/>
     </row>
     <row r="32" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="18"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="12"/>
     </row>
     <row r="33" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="21"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2339,7 +2342,7 @@
     <mergeCell ref="F1:L1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>

</xml_diff>